<commit_message>
adding test cases complying OWASP
</commit_message>
<xml_diff>
--- a/test_case/html_injection/2. TC_HTML_Injection.xlsx
+++ b/test_case/html_injection/2. TC_HTML_Injection.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitProjects\pnt-stqa-training\test-case-bwapp-pntb24\test_case\html_injection\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE646F5C-0C4C-483B-A0B0-317A79A2B336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74F9DA33-75F8-4C00-B6C0-791EDB4CB74E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="36">
   <si>
     <t>TC ID</t>
   </si>
@@ -161,6 +161,9 @@
   </si>
   <si>
     <t>Text has appeared as italic text, not plan</t>
+  </si>
+  <si>
+    <t>The text "SROLLED _TEXT" will not be displayed and scrolled from right to left</t>
   </si>
 </sst>
 </file>
@@ -565,8 +568,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+    <sheetView tabSelected="1" topLeftCell="D6" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -660,7 +663,9 @@
       <c r="E5" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="10"/>
+      <c r="F5" s="10" t="s">
+        <v>21</v>
+      </c>
       <c r="G5" s="10" t="s">
         <v>27</v>
       </c>
@@ -683,7 +688,9 @@
       <c r="E6" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="F6" s="10"/>
+      <c r="F6" s="10" t="s">
+        <v>35</v>
+      </c>
       <c r="G6" s="10" t="s">
         <v>30</v>
       </c>

</xml_diff>